<commit_message>
More Additions to Lemma List
Things I am unsure about are highlighted with yellow.
</commit_message>
<xml_diff>
--- a/lemmatizer/lemma_list.xlsx
+++ b/lemmatizer/lemma_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="340" windowWidth="21540" windowHeight="12320"/>
+    <workbookView xWindow="260" yWindow="1800" windowWidth="21540" windowHeight="12320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19648" uniqueCount="4997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19645" uniqueCount="5031">
   <si>
     <t>V</t>
   </si>
@@ -14993,9 +14993,6 @@
     <t>be happy/examine</t>
   </si>
   <si>
-    <t>ϫⲁ(ⲁ)ϫⲉ</t>
-  </si>
-  <si>
     <t>ϫⲓ/ϫⲟ</t>
   </si>
   <si>
@@ -15012,13 +15009,118 @@
   </si>
   <si>
     <t>lay down</t>
+  </si>
+  <si>
+    <t>ϭⲱⲱⲗⲉ</t>
+  </si>
+  <si>
+    <t>ϭⲱⲗⲡ̄</t>
+  </si>
+  <si>
+    <t>ϭⲱϫⲃ̄</t>
+  </si>
+  <si>
+    <t>ϭⲱⲛⲧ̄</t>
+  </si>
+  <si>
+    <t>ⲧⲥ̄ⲧⲟ</t>
+  </si>
+  <si>
+    <t>ⲧⲥ̄ⲧⲉ</t>
+  </si>
+  <si>
+    <t>ⲧⲥ̄ⲓⲟ</t>
+  </si>
+  <si>
+    <t>ⲧⲥ̄ⲓⲉ</t>
+  </si>
+  <si>
+    <t>ⲱⲙⲥ̄</t>
+  </si>
+  <si>
+    <t>ⲱⲙⲕ̄</t>
+  </si>
+  <si>
+    <t>ⲱⲗ</t>
+  </si>
+  <si>
+    <t>ⲱⲕⲙ̄</t>
+  </si>
+  <si>
+    <t>ⲱϥⲉ</t>
+  </si>
+  <si>
+    <t>ⲱⲃϣ̄</t>
+  </si>
+  <si>
+    <t>ⲱϭⲧ̄</t>
+  </si>
+  <si>
+    <t>ⲱϩⲥ̄</t>
+  </si>
+  <si>
+    <t>ⲱϥⲧ̄</t>
+  </si>
+  <si>
+    <t>ⲱϣⲙ̄</t>
+  </si>
+  <si>
+    <t>ⲛ̄ⲧⲛ̄</t>
+  </si>
+  <si>
+    <t>ⲛⲟⲩϭⲥ̄</t>
+  </si>
+  <si>
+    <t>ⲛⲟⲩϣⲡ̄</t>
+  </si>
+  <si>
+    <t>ⲛⲁϩⲣⲏⲛ̄</t>
+  </si>
+  <si>
+    <t>ⲛⲉⲥⲉ</t>
+  </si>
+  <si>
+    <t>ⲛⲟⲩϩⲙ̄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ⲛⲟⲩϩⲙ̄ </t>
+  </si>
+  <si>
+    <t>ⲛⲁϩⲣⲛ̄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ⲛⲟⲩϩⲙ </t>
+  </si>
+  <si>
+    <t>ⲛ̄ϣⲟⲧ</t>
+  </si>
+  <si>
+    <t>ϩⲛ̄</t>
+  </si>
+  <si>
+    <t>ⲁⲗⲉ? Ⲗⲟ?</t>
+  </si>
+  <si>
+    <t>ⲁϫⲛ̄</t>
+  </si>
+  <si>
+    <t>ⲕⲱⲣϣ̄</t>
+  </si>
+  <si>
+    <t>ⲁⲥⲁⲓ</t>
+  </si>
+  <si>
+    <t>ⲃⲁⲁⲃⲉ</t>
+  </si>
+  <si>
+    <t>ⲃⲱⲧⲉ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15066,8 +15168,12 @@
       <color rgb="FF000000"/>
       <name val="Antinoou"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Antinoou"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15077,12 +15183,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15161,14 +15261,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -15535,8 +15636,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H5245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+    <sheetView tabSelected="1" topLeftCell="A578" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D545" sqref="D545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -18239,8 +18340,8 @@
       <c r="C138" t="s">
         <v>39</v>
       </c>
-      <c r="D138" s="5" t="s">
-        <v>4990</v>
+      <c r="D138" s="6" t="s">
+        <v>631</v>
       </c>
       <c r="G138" t="s">
         <v>4782</v>
@@ -18328,7 +18429,7 @@
         <v>0</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>4991</v>
+        <v>4990</v>
       </c>
       <c r="G143" t="s">
         <v>4756</v>
@@ -18481,10 +18582,10 @@
         <v>0</v>
       </c>
       <c r="D152" s="1" t="s">
+        <v>4991</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>4992</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>4993</v>
       </c>
       <c r="G152" t="s">
         <v>4756</v>
@@ -18586,7 +18687,7 @@
         <v>0</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>4994</v>
+        <v>4993</v>
       </c>
       <c r="G158" t="s">
         <v>4838</v>
@@ -18671,7 +18772,7 @@
         <v>0</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>4995</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -18807,7 +18908,7 @@
         <v>739</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>4996</v>
+        <v>4995</v>
       </c>
       <c r="G171" t="s">
         <v>4787</v>
@@ -18908,7 +19009,7 @@
       <c r="C177" t="s">
         <v>0</v>
       </c>
-      <c r="D177" s="1" t="s">
+      <c r="D177" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G177" t="s">
@@ -18926,7 +19027,7 @@
         <v>39</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>1</v>
+        <v>853</v>
       </c>
       <c r="G178" t="s">
         <v>4782</v>
@@ -18943,7 +19044,7 @@
         <v>0</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>1</v>
+        <v>4996</v>
       </c>
       <c r="G179" t="s">
         <v>4756</v>
@@ -18960,7 +19061,7 @@
         <v>0</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>1</v>
+        <v>4997</v>
       </c>
       <c r="G180" t="s">
         <v>4756</v>
@@ -18977,7 +19078,7 @@
         <v>0</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="G181" t="s">
         <v>4756</v>
@@ -18994,7 +19095,7 @@
         <v>0</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="G182" t="s">
         <v>4756</v>
@@ -19011,7 +19112,7 @@
         <v>0</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="G183" t="s">
         <v>4838</v>
@@ -19028,7 +19129,7 @@
         <v>0</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1</v>
+        <v>860</v>
       </c>
       <c r="G184" t="s">
         <v>4756</v>
@@ -19045,7 +19146,7 @@
         <v>39</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1</v>
+        <v>860</v>
       </c>
       <c r="G185" t="s">
         <v>4782</v>
@@ -19062,7 +19163,7 @@
         <v>39</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1</v>
+        <v>859</v>
       </c>
       <c r="G186" t="s">
         <v>4782</v>
@@ -19079,7 +19180,7 @@
         <v>0</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -19093,7 +19194,7 @@
         <v>0</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>1</v>
+        <v>4997</v>
       </c>
       <c r="G188" t="s">
         <v>4756</v>
@@ -19109,7 +19210,7 @@
       <c r="C189" t="s">
         <v>0</v>
       </c>
-      <c r="D189" s="1" t="s">
+      <c r="D189" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G189" t="s">
@@ -19127,7 +19228,7 @@
         <v>0</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="G190" t="s">
         <v>4756</v>
@@ -19144,7 +19245,7 @@
         <v>0</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="G191" t="s">
         <v>4756</v>
@@ -19161,7 +19262,7 @@
         <v>0</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="G192" t="s">
         <v>4756</v>
@@ -19177,7 +19278,7 @@
       <c r="C193" t="s">
         <v>0</v>
       </c>
-      <c r="D193" s="1" t="s">
+      <c r="D193" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G193" t="s">
@@ -19195,7 +19296,7 @@
         <v>0</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="G194" t="s">
         <v>4838</v>
@@ -19212,7 +19313,7 @@
         <v>39</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>1</v>
+        <v>4998</v>
       </c>
       <c r="G195" t="s">
         <v>4782</v>
@@ -19229,7 +19330,7 @@
         <v>39</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>1</v>
+        <v>4998</v>
       </c>
       <c r="G196" t="s">
         <v>4782</v>
@@ -19246,7 +19347,7 @@
         <v>0</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1</v>
+        <v>4997</v>
       </c>
       <c r="G197" t="s">
         <v>4837</v>
@@ -19263,7 +19364,7 @@
         <v>39</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>1</v>
+        <v>4997</v>
       </c>
       <c r="G198" t="s">
         <v>4837</v>
@@ -19280,7 +19381,7 @@
         <v>39</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1</v>
+        <v>4999</v>
       </c>
       <c r="G199" t="s">
         <v>4782</v>
@@ -19297,7 +19398,7 @@
         <v>0</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>1</v>
+        <v>4996</v>
       </c>
       <c r="G200" t="s">
         <v>4837</v>
@@ -19314,7 +19415,7 @@
         <v>39</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>1</v>
+        <v>4996</v>
       </c>
       <c r="G201" t="s">
         <v>4837</v>
@@ -19331,7 +19432,7 @@
         <v>0</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>1</v>
+        <v>860</v>
       </c>
       <c r="G202" t="s">
         <v>4838</v>
@@ -19348,7 +19449,7 @@
         <v>0</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1</v>
+        <v>5027</v>
       </c>
       <c r="G203" t="s">
         <v>4838</v>
@@ -19364,7 +19465,7 @@
       <c r="C204" t="s">
         <v>39</v>
       </c>
-      <c r="D204" s="1" t="s">
+      <c r="D204" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G204" t="s">
@@ -19382,7 +19483,7 @@
         <v>0</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>1</v>
+        <v>869</v>
       </c>
       <c r="G205" t="s">
         <v>4838</v>
@@ -19399,7 +19500,7 @@
         <v>0</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>1</v>
+        <v>869</v>
       </c>
       <c r="G206" t="s">
         <v>4756</v>
@@ -19416,7 +19517,7 @@
         <v>0</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1</v>
+        <v>869</v>
       </c>
       <c r="G207" t="s">
         <v>4838</v>
@@ -19433,7 +19534,7 @@
         <v>0</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1</v>
+        <v>869</v>
       </c>
       <c r="G208" t="s">
         <v>4838</v>
@@ -19450,7 +19551,7 @@
         <v>39</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1</v>
+        <v>1587</v>
       </c>
       <c r="G209" t="s">
         <v>4782</v>
@@ -19467,7 +19568,7 @@
         <v>0</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1</v>
+        <v>1587</v>
       </c>
       <c r="G210" t="s">
         <v>4838</v>
@@ -19484,7 +19585,7 @@
         <v>0</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>1</v>
+        <v>4577</v>
       </c>
       <c r="G211" t="s">
         <v>4838</v>
@@ -19501,7 +19602,7 @@
         <v>275</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1</v>
+        <v>927</v>
       </c>
       <c r="G212" t="s">
         <v>4783</v>
@@ -19518,7 +19619,7 @@
         <v>275</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1</v>
+        <v>927</v>
       </c>
       <c r="G213" t="s">
         <v>4783</v>
@@ -19535,7 +19636,7 @@
         <v>24</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1</v>
+        <v>5026</v>
       </c>
       <c r="G214" t="s">
         <v>4824</v>
@@ -19552,7 +19653,7 @@
         <v>0</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
       <c r="G215" t="s">
         <v>4838</v>
@@ -19568,8 +19669,8 @@
       <c r="C216" t="s">
         <v>0</v>
       </c>
-      <c r="D216" s="1" t="s">
-        <v>1</v>
+      <c r="D216" s="5" t="s">
+        <v>1613</v>
       </c>
       <c r="G216" t="s">
         <v>4838</v>
@@ -19586,7 +19687,7 @@
         <v>39</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1</v>
+        <v>1021</v>
       </c>
       <c r="G217" t="s">
         <v>4782</v>
@@ -19602,8 +19703,8 @@
       <c r="C218" t="s">
         <v>932</v>
       </c>
-      <c r="D218" s="1" t="s">
-        <v>1</v>
+      <c r="D218" s="5" t="s">
+        <v>5025</v>
       </c>
       <c r="G218" t="s">
         <v>4847</v>
@@ -19620,7 +19721,7 @@
         <v>932</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1</v>
+        <v>1585</v>
       </c>
       <c r="G219" t="s">
         <v>4848</v>
@@ -19637,7 +19738,7 @@
         <v>932</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>1</v>
+        <v>1585</v>
       </c>
       <c r="G220" t="s">
         <v>4848</v>
@@ -19654,7 +19755,7 @@
         <v>932</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1</v>
+        <v>1585</v>
       </c>
       <c r="G221" t="s">
         <v>4848</v>
@@ -19671,7 +19772,7 @@
         <v>932</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1</v>
+        <v>1585</v>
       </c>
       <c r="G222" t="s">
         <v>4848</v>
@@ -19688,7 +19789,7 @@
         <v>932</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1</v>
+        <v>1585</v>
       </c>
       <c r="G223" t="s">
         <v>4848</v>
@@ -19705,7 +19806,7 @@
         <v>932</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1</v>
+        <v>1585</v>
       </c>
       <c r="G224" t="s">
         <v>4848</v>
@@ -19721,8 +19822,8 @@
       <c r="C225" t="s">
         <v>932</v>
       </c>
-      <c r="D225" s="1" t="s">
-        <v>1</v>
+      <c r="D225" s="5" t="s">
+        <v>1585</v>
       </c>
       <c r="G225" t="s">
         <v>4848</v>
@@ -19739,7 +19840,7 @@
         <v>932</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1</v>
+        <v>2965</v>
       </c>
       <c r="G226" t="s">
         <v>4848</v>
@@ -19756,7 +19857,7 @@
         <v>932</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1</v>
+        <v>1607</v>
       </c>
       <c r="G227" t="s">
         <v>4847</v>
@@ -19773,7 +19874,7 @@
         <v>932</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
       <c r="G228" t="s">
         <v>4848</v>
@@ -19790,7 +19891,7 @@
         <v>39</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1</v>
+        <v>5028</v>
       </c>
       <c r="G229" t="s">
         <v>4782</v>
@@ -19807,7 +19908,7 @@
         <v>0</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1</v>
+        <v>5029</v>
       </c>
       <c r="G230" t="s">
         <v>4838</v>
@@ -19824,7 +19925,7 @@
         <v>0</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1</v>
+        <v>1386</v>
       </c>
       <c r="G231" t="s">
         <v>4756</v>
@@ -19841,7 +19942,7 @@
         <v>0</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>1</v>
+        <v>5030</v>
       </c>
       <c r="G232" t="s">
         <v>4756</v>
@@ -19858,7 +19959,7 @@
         <v>39</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1</v>
+        <v>1385</v>
       </c>
       <c r="G233" t="s">
         <v>4782</v>
@@ -19875,7 +19976,7 @@
         <v>39</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>1</v>
+        <v>1386</v>
       </c>
       <c r="G234" t="s">
         <v>4782</v>
@@ -19892,7 +19993,7 @@
         <v>39</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1</v>
+        <v>5030</v>
       </c>
       <c r="G235" t="s">
         <v>4782</v>
@@ -19909,7 +20010,7 @@
         <v>0</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1</v>
+        <v>1383</v>
       </c>
       <c r="G236" t="s">
         <v>4838</v>
@@ -19925,8 +20026,8 @@
       <c r="C237" t="s">
         <v>0</v>
       </c>
-      <c r="D237" s="1" t="s">
-        <v>1</v>
+      <c r="D237" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="G237" t="s">
         <v>4838</v>
@@ -19943,7 +20044,7 @@
         <v>0</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>1</v>
+        <v>1386</v>
       </c>
       <c r="G238" t="s">
         <v>4792</v>
@@ -19959,9 +20060,7 @@
       <c r="C239" t="s">
         <v>0</v>
       </c>
-      <c r="D239" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="D239" s="5"/>
     </row>
     <row r="240" spans="1:7">
       <c r="A240">
@@ -19974,7 +20073,7 @@
         <v>0</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>1</v>
+        <v>1389</v>
       </c>
       <c r="G240" t="s">
         <v>4838</v>
@@ -19991,7 +20090,7 @@
         <v>0</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1</v>
+        <v>5030</v>
       </c>
       <c r="G241" t="s">
         <v>4838</v>
@@ -20008,7 +20107,7 @@
         <v>0</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>1</v>
+        <v>1385</v>
       </c>
       <c r="G242" t="s">
         <v>4842</v>
@@ -20025,7 +20124,7 @@
         <v>0</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G243" t="s">
         <v>4756</v>
@@ -20042,7 +20141,7 @@
         <v>0</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G244" t="s">
         <v>4836</v>
@@ -20059,7 +20158,7 @@
         <v>0</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>1</v>
+        <v>1587</v>
       </c>
       <c r="G245" t="s">
         <v>4756</v>
@@ -20075,7 +20174,7 @@
       <c r="C246" t="s">
         <v>0</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="D246" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G246" t="s">
@@ -20092,9 +20191,6 @@
       <c r="C247" t="s">
         <v>275</v>
       </c>
-      <c r="D247" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G247" t="s">
         <v>4783</v>
       </c>
@@ -21968,7 +22064,7 @@
         <v>0</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>1</v>
+        <v>1607</v>
       </c>
       <c r="G358" t="s">
         <v>4727</v>
@@ -21985,7 +22081,7 @@
         <v>24</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>1</v>
+        <v>5024</v>
       </c>
       <c r="G359" t="s">
         <v>4824</v>
@@ -22002,7 +22098,7 @@
         <v>24</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>1</v>
+        <v>5024</v>
       </c>
       <c r="G360" t="s">
         <v>4824</v>
@@ -22019,7 +22115,7 @@
         <v>39</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>1</v>
+        <v>2948</v>
       </c>
       <c r="G361" t="s">
         <v>4782</v>
@@ -22036,7 +22132,7 @@
         <v>24</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>1</v>
+        <v>5024</v>
       </c>
     </row>
     <row r="363" spans="1:7">
@@ -22050,7 +22146,7 @@
         <v>0</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>1</v>
+        <v>2931</v>
       </c>
       <c r="G363" t="s">
         <v>4765</v>
@@ -22067,7 +22163,7 @@
         <v>39</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>1</v>
+        <v>2931</v>
       </c>
       <c r="G364" t="s">
         <v>4765</v>
@@ -22084,7 +22180,7 @@
         <v>275</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>1</v>
+        <v>2933</v>
       </c>
       <c r="G365" t="s">
         <v>4846</v>
@@ -22101,7 +22197,7 @@
         <v>39</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>1</v>
+        <v>5023</v>
       </c>
       <c r="G366" t="s">
         <v>4782</v>
@@ -22118,7 +22214,7 @@
         <v>0</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>1</v>
+        <v>5022</v>
       </c>
       <c r="G367" t="s">
         <v>4838</v>
@@ -22134,8 +22230,8 @@
       <c r="C368" t="s">
         <v>0</v>
       </c>
-      <c r="D368" s="1" t="s">
-        <v>1</v>
+      <c r="D368" s="5" t="s">
+        <v>3084</v>
       </c>
       <c r="G368" t="s">
         <v>4838</v>
@@ -22151,8 +22247,8 @@
       <c r="C369" t="s">
         <v>0</v>
       </c>
-      <c r="D369" s="1" t="s">
-        <v>1</v>
+      <c r="D369" s="5" t="s">
+        <v>3084</v>
       </c>
       <c r="G369" t="s">
         <v>4838</v>
@@ -22169,7 +22265,7 @@
         <v>24</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>1</v>
+        <v>5021</v>
       </c>
       <c r="G370" t="s">
         <v>4824</v>
@@ -22185,8 +22281,8 @@
       <c r="C371" t="s">
         <v>0</v>
       </c>
-      <c r="D371" s="1" t="s">
-        <v>1</v>
+      <c r="D371" s="5" t="s">
+        <v>2948</v>
       </c>
       <c r="G371" t="s">
         <v>4838</v>
@@ -22203,7 +22299,7 @@
         <v>275</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>1</v>
+        <v>1589</v>
       </c>
       <c r="G372" t="s">
         <v>4783</v>
@@ -22220,7 +22316,7 @@
         <v>0</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>1</v>
+        <v>2965</v>
       </c>
       <c r="G373" t="s">
         <v>4770</v>
@@ -22237,7 +22333,7 @@
         <v>0</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>1</v>
+        <v>3083</v>
       </c>
       <c r="G374" t="s">
         <v>4800</v>
@@ -22254,7 +22350,7 @@
         <v>0</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>1</v>
+        <v>5020</v>
       </c>
       <c r="G375" t="s">
         <v>4756</v>
@@ -22271,7 +22367,7 @@
         <v>0</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>1</v>
+        <v>5019</v>
       </c>
       <c r="G376" t="s">
         <v>4756</v>
@@ -22288,7 +22384,7 @@
         <v>0</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>1</v>
+        <v>3086</v>
       </c>
       <c r="G377" t="s">
         <v>4756</v>
@@ -22305,7 +22401,7 @@
         <v>0</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>1</v>
+        <v>3058</v>
       </c>
       <c r="G378" t="s">
         <v>4838</v>
@@ -22321,7 +22417,7 @@
       <c r="C379" t="s">
         <v>0</v>
       </c>
-      <c r="D379" s="1" t="s">
+      <c r="D379" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -22336,7 +22432,7 @@
         <v>275</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>1</v>
+        <v>5018</v>
       </c>
       <c r="G380" t="s">
         <v>4783</v>
@@ -22353,7 +22449,7 @@
         <v>39</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>1</v>
+        <v>3086</v>
       </c>
       <c r="G381" t="s">
         <v>4782</v>
@@ -22370,7 +22466,7 @@
         <v>39</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>1</v>
+        <v>1585</v>
       </c>
       <c r="G382" t="s">
         <v>4782</v>
@@ -22387,7 +22483,7 @@
         <v>24</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>1</v>
+        <v>5017</v>
       </c>
       <c r="G383" t="s">
         <v>4824</v>
@@ -22404,7 +22500,7 @@
         <v>24</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>1</v>
+        <v>5017</v>
       </c>
       <c r="G384" t="s">
         <v>4824</v>
@@ -22421,7 +22517,7 @@
         <v>0</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>1</v>
+        <v>5016</v>
       </c>
       <c r="G385" t="s">
         <v>4838</v>
@@ -22438,7 +22534,7 @@
         <v>0</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>1</v>
+        <v>3086</v>
       </c>
       <c r="G386" t="s">
         <v>4838</v>
@@ -22455,7 +22551,7 @@
         <v>39</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>1</v>
+        <v>5015</v>
       </c>
       <c r="G387" t="s">
         <v>4782</v>
@@ -22472,7 +22568,7 @@
         <v>0</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>1</v>
+        <v>3078</v>
       </c>
       <c r="G388" t="s">
         <v>4822</v>
@@ -22489,7 +22585,7 @@
         <v>0</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>1</v>
+        <v>3083</v>
       </c>
       <c r="G389" t="s">
         <v>4756</v>
@@ -22505,7 +22601,7 @@
       <c r="C390" t="s">
         <v>24</v>
       </c>
-      <c r="D390" s="1" t="s">
+      <c r="D390" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G390" t="s">
@@ -22522,7 +22618,7 @@
       <c r="C391" t="s">
         <v>24</v>
       </c>
-      <c r="D391" s="1" t="s">
+      <c r="D391" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G391" t="s">
@@ -22539,7 +22635,7 @@
       <c r="C392" t="s">
         <v>0</v>
       </c>
-      <c r="D392" s="1" t="s">
+      <c r="D392" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G392" t="s">
@@ -22557,7 +22653,7 @@
         <v>24</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>1</v>
+        <v>5014</v>
       </c>
       <c r="G393" t="s">
         <v>4824</v>
@@ -22573,8 +22669,8 @@
       <c r="C394" t="s">
         <v>39</v>
       </c>
-      <c r="D394" s="1" t="s">
-        <v>1</v>
+      <c r="D394" s="6" t="s">
+        <v>1613</v>
       </c>
       <c r="G394" t="s">
         <v>4782</v>
@@ -22591,7 +22687,7 @@
         <v>0</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1</v>
+        <v>4575</v>
       </c>
       <c r="G395" t="s">
         <v>4837</v>
@@ -22608,7 +22704,7 @@
         <v>39</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>1</v>
+        <v>4575</v>
       </c>
       <c r="G396" t="s">
         <v>4837</v>
@@ -22624,7 +22720,7 @@
       <c r="C397" t="s">
         <v>0</v>
       </c>
-      <c r="D397" s="1" t="s">
+      <c r="D397" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G397" t="s">
@@ -22641,8 +22737,8 @@
       <c r="C398" t="s">
         <v>0</v>
       </c>
-      <c r="D398" s="1" t="s">
-        <v>1</v>
+      <c r="D398" s="6" t="s">
+        <v>5013</v>
       </c>
       <c r="G398" t="s">
         <v>4838</v>
@@ -22658,7 +22754,7 @@
       <c r="C399" t="s">
         <v>0</v>
       </c>
-      <c r="D399" s="1" t="s">
+      <c r="D399" s="7" t="s">
         <v>1</v>
       </c>
       <c r="G399" t="s">
@@ -22676,7 +22772,7 @@
         <v>39</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>1</v>
+        <v>5012</v>
       </c>
       <c r="G400" t="s">
         <v>4782</v>
@@ -22693,7 +22789,7 @@
         <v>0</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>1</v>
+        <v>5011</v>
       </c>
       <c r="G401" t="s">
         <v>4838</v>
@@ -22710,7 +22806,7 @@
         <v>0</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>1</v>
+        <v>5010</v>
       </c>
       <c r="G402" t="s">
         <v>4838</v>
@@ -22727,7 +22823,7 @@
         <v>0</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>1</v>
+        <v>5009</v>
       </c>
       <c r="G403" t="s">
         <v>4838</v>
@@ -22744,7 +22840,7 @@
         <v>39</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>1</v>
+        <v>5008</v>
       </c>
       <c r="G404" t="s">
         <v>4782</v>
@@ -22761,7 +22857,7 @@
         <v>39</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>1</v>
+        <v>5007</v>
       </c>
       <c r="G405" t="s">
         <v>4782</v>
@@ -22778,7 +22874,7 @@
         <v>0</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>1</v>
+        <v>5006</v>
       </c>
       <c r="G406" t="s">
         <v>4838</v>
@@ -22795,7 +22891,7 @@
         <v>0</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>1</v>
+        <v>5005</v>
       </c>
       <c r="G407" t="s">
         <v>4838</v>
@@ -22812,7 +22908,7 @@
         <v>0</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>1</v>
+        <v>5004</v>
       </c>
       <c r="G408" t="s">
         <v>4838</v>
@@ -23200,7 +23296,7 @@
         <v>39</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>1</v>
+        <v>3301</v>
       </c>
       <c r="G431" t="s">
         <v>4782</v>
@@ -23931,7 +24027,7 @@
         <v>0</v>
       </c>
       <c r="D474" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
       <c r="G474" t="s">
         <v>4756</v>
@@ -23948,7 +24044,7 @@
         <v>0</v>
       </c>
       <c r="D475" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="476" spans="1:7">
@@ -23962,7 +24058,7 @@
         <v>0</v>
       </c>
       <c r="D476" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
       <c r="G476" t="s">
         <v>4756</v>
@@ -23979,7 +24075,7 @@
         <v>0</v>
       </c>
       <c r="D477" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
       <c r="G477" t="s">
         <v>4838</v>
@@ -23996,7 +24092,7 @@
         <v>0</v>
       </c>
       <c r="D478" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="479" spans="1:7">
@@ -25019,7 +25115,7 @@
         <v>2</v>
       </c>
       <c r="D538" s="1" t="s">
-        <v>1</v>
+        <v>3980</v>
       </c>
       <c r="G538" t="s">
         <v>4768</v>
@@ -26019,7 +26115,7 @@
         <v>39</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>1</v>
+        <v>4191</v>
       </c>
       <c r="G597" t="s">
         <v>4782</v>
@@ -26049,9 +26145,6 @@
       <c r="C599" t="s">
         <v>39</v>
       </c>
-      <c r="D599" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G599" t="s">
         <v>4782</v>
       </c>
@@ -27197,7 +27290,7 @@
         <v>0</v>
       </c>
       <c r="D667" s="1" t="s">
-        <v>1</v>
+        <v>4379</v>
       </c>
       <c r="G667" t="s">
         <v>4756</v>
@@ -27214,7 +27307,7 @@
         <v>0</v>
       </c>
       <c r="D668" s="1" t="s">
-        <v>1</v>
+        <v>4379</v>
       </c>
       <c r="G668" t="s">
         <v>4787</v>
@@ -27231,7 +27324,7 @@
         <v>2</v>
       </c>
       <c r="D669" s="1" t="s">
-        <v>1</v>
+        <v>4383</v>
       </c>
       <c r="G669" t="s">
         <v>4768</v>
@@ -27248,7 +27341,7 @@
         <v>2</v>
       </c>
       <c r="D670" s="1" t="s">
-        <v>1</v>
+        <v>4383</v>
       </c>
       <c r="G670" t="s">
         <v>4768</v>
@@ -27264,7 +27357,7 @@
       <c r="C671" t="s">
         <v>0</v>
       </c>
-      <c r="D671" s="1" t="s">
+      <c r="D671" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G671" t="s">
@@ -27281,7 +27374,7 @@
       <c r="C672" t="s">
         <v>0</v>
       </c>
-      <c r="D672" s="1" t="s">
+      <c r="D672" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G672" t="s">
@@ -27299,7 +27392,7 @@
         <v>0</v>
       </c>
       <c r="D673" s="1" t="s">
-        <v>1</v>
+        <v>4395</v>
       </c>
       <c r="G673" t="s">
         <v>4787</v>
@@ -27316,7 +27409,7 @@
         <v>0</v>
       </c>
       <c r="D674" s="1" t="s">
-        <v>1</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="675" spans="1:7">
@@ -27330,7 +27423,7 @@
         <v>0</v>
       </c>
       <c r="D675" s="1" t="s">
-        <v>1</v>
+        <v>4399</v>
       </c>
       <c r="G675" t="s">
         <v>4756</v>
@@ -27347,7 +27440,7 @@
         <v>0</v>
       </c>
       <c r="D676" s="1" t="s">
-        <v>1</v>
+        <v>4399</v>
       </c>
       <c r="G676" t="s">
         <v>4838</v>
@@ -27363,7 +27456,7 @@
       <c r="C677" t="s">
         <v>0</v>
       </c>
-      <c r="D677" s="1" t="s">
+      <c r="D677" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G677" t="s">
@@ -27380,7 +27473,7 @@
       <c r="C678" t="s">
         <v>0</v>
       </c>
-      <c r="D678" s="1" t="s">
+      <c r="D678" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G678" t="s">
@@ -27398,7 +27491,7 @@
         <v>0</v>
       </c>
       <c r="D679" s="1" t="s">
-        <v>1</v>
+        <v>5003</v>
       </c>
       <c r="G679" t="s">
         <v>4756</v>
@@ -27415,7 +27508,7 @@
         <v>0</v>
       </c>
       <c r="D680" s="1" t="s">
-        <v>1</v>
+        <v>5002</v>
       </c>
       <c r="G680" t="s">
         <v>4787</v>
@@ -27432,7 +27525,7 @@
         <v>0</v>
       </c>
       <c r="D681" s="1" t="s">
-        <v>1</v>
+        <v>5001</v>
       </c>
       <c r="G681" t="s">
         <v>4756</v>
@@ -27449,7 +27542,7 @@
         <v>39</v>
       </c>
       <c r="D682" s="1" t="s">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="G682" t="s">
         <v>4782</v>
@@ -27465,8 +27558,8 @@
       <c r="C683" t="s">
         <v>0</v>
       </c>
-      <c r="D683" s="1" t="s">
-        <v>1</v>
+      <c r="D683" s="5" t="s">
+        <v>4432</v>
       </c>
       <c r="G683" t="s">
         <v>4838</v>
@@ -27483,7 +27576,7 @@
         <v>2</v>
       </c>
       <c r="D684" s="1" t="s">
-        <v>1</v>
+        <v>4437</v>
       </c>
       <c r="G684" t="s">
         <v>4729</v>
@@ -27500,7 +27593,7 @@
         <v>2</v>
       </c>
       <c r="D685" s="1" t="s">
-        <v>1</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="686" spans="1:7">
@@ -27514,7 +27607,7 @@
         <v>0</v>
       </c>
       <c r="D686" s="1" t="s">
-        <v>1</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="687" spans="1:7">
@@ -27527,7 +27620,7 @@
       <c r="C687" t="s">
         <v>2</v>
       </c>
-      <c r="D687" s="1" t="s">
+      <c r="D687" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G687" t="s">
@@ -27545,7 +27638,7 @@
         <v>2</v>
       </c>
       <c r="D688" s="1" t="s">
-        <v>1</v>
+        <v>3201</v>
       </c>
       <c r="G688" t="s">
         <v>4768</v>
@@ -27562,7 +27655,7 @@
         <v>2</v>
       </c>
       <c r="D689" s="1" t="s">
-        <v>1</v>
+        <v>3267</v>
       </c>
     </row>
     <row r="690" spans="1:6">
@@ -27576,7 +27669,7 @@
         <v>0</v>
       </c>
       <c r="D690" s="1" t="s">
-        <v>1</v>
+        <v>205</v>
       </c>
     </row>
     <row r="691" spans="1:6">

</xml_diff>

<commit_message>
More Additions to Lemmatizer
I’ve done everything I feel sure about at this point, and have left
many cells highlighted. I need further guidance to finish.
</commit_message>
<xml_diff>
--- a/lemmatizer/lemma_list.xlsx
+++ b/lemmatizer/lemma_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19643" uniqueCount="5027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19643" uniqueCount="5034">
   <si>
     <t>V</t>
   </si>
@@ -15102,6 +15102,27 @@
   </si>
   <si>
     <t>ⲙⲟⲩϫϭ</t>
+  </si>
+  <si>
+    <t>ⲱⲣⲃ</t>
+  </si>
+  <si>
+    <t>ⲉⲧⲛ</t>
+  </si>
+  <si>
+    <t>ⲧϩⲡⲟ</t>
+  </si>
+  <si>
+    <t>ⲧⲡⲣϣⲟ</t>
+  </si>
+  <si>
+    <t>ⲕⲱⲕ</t>
+  </si>
+  <si>
+    <t>ⲗⲱϫⲧ</t>
+  </si>
+  <si>
+    <t>ⲙⲟⲩⲛ</t>
   </si>
 </sst>
 </file>
@@ -15624,8 +15645,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H5245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D230" sqref="D230"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -20179,6 +20200,9 @@
       <c r="C247" t="s">
         <v>275</v>
       </c>
+      <c r="D247" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="G247" t="s">
         <v>4783</v>
       </c>
@@ -20194,7 +20218,7 @@
         <v>275</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1</v>
+        <v>457</v>
       </c>
       <c r="G248" t="s">
         <v>4846</v>
@@ -20211,7 +20235,7 @@
         <v>24</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1</v>
+        <v>477</v>
       </c>
       <c r="G249" t="s">
         <v>4824</v>
@@ -20227,7 +20251,7 @@
       <c r="C250" t="s">
         <v>24</v>
       </c>
-      <c r="D250" s="1" t="s">
+      <c r="D250" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G250" t="s">
@@ -20245,7 +20269,7 @@
         <v>24</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1</v>
+        <v>934</v>
       </c>
       <c r="G251" t="s">
         <v>4824</v>
@@ -20262,7 +20286,7 @@
         <v>24</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>1</v>
+        <v>1557</v>
       </c>
       <c r="G252" t="s">
         <v>4824</v>
@@ -20279,7 +20303,7 @@
         <v>0</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>1</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -20292,7 +20316,7 @@
       <c r="C254" t="s">
         <v>0</v>
       </c>
-      <c r="D254" s="1" t="s">
+      <c r="D254" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G254" t="s">
@@ -20309,7 +20333,7 @@
       <c r="C255" t="s">
         <v>39</v>
       </c>
-      <c r="D255" s="1" t="s">
+      <c r="D255" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G255" t="s">
@@ -20326,7 +20350,7 @@
       <c r="C256" t="s">
         <v>0</v>
       </c>
-      <c r="D256" s="1" t="s">
+      <c r="D256" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -20340,7 +20364,7 @@
       <c r="C257" t="s">
         <v>0</v>
       </c>
-      <c r="D257" s="1" t="s">
+      <c r="D257" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -20355,7 +20379,7 @@
         <v>0</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>1</v>
+        <v>1613</v>
       </c>
       <c r="G258" t="s">
         <v>4756</v>
@@ -20371,7 +20395,7 @@
       <c r="C259" t="s">
         <v>0</v>
       </c>
-      <c r="D259" s="1" t="s">
+      <c r="D259" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G259" t="s">
@@ -20388,7 +20412,7 @@
       <c r="C260" t="s">
         <v>24</v>
       </c>
-      <c r="D260" s="1" t="s">
+      <c r="D260" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G260" t="s">
@@ -20405,7 +20429,7 @@
       <c r="C261" t="s">
         <v>0</v>
       </c>
-      <c r="D261" s="1" t="s">
+      <c r="D261" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G261" t="s">
@@ -20422,7 +20446,7 @@
       <c r="C262" t="s">
         <v>0</v>
       </c>
-      <c r="D262" s="1" t="s">
+      <c r="D262" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G262" t="s">
@@ -20440,7 +20464,7 @@
         <v>24</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>1</v>
+        <v>1774</v>
       </c>
       <c r="G263" t="s">
         <v>4824</v>
@@ -20457,7 +20481,7 @@
         <v>24</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>1</v>
+        <v>1774</v>
       </c>
       <c r="G264" t="s">
         <v>4824</v>
@@ -20474,7 +20498,7 @@
         <v>0</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>1</v>
+        <v>5027</v>
       </c>
       <c r="G265" t="s">
         <v>4756</v>
@@ -20490,9 +20514,7 @@
       <c r="C266" t="s">
         <v>24</v>
       </c>
-      <c r="D266" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="D266" s="5"/>
       <c r="G266" t="s">
         <v>4824</v>
       </c>
@@ -20507,7 +20529,7 @@
       <c r="C267" t="s">
         <v>24</v>
       </c>
-      <c r="D267" s="1" t="s">
+      <c r="D267" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G267" t="s">
@@ -20525,7 +20547,7 @@
         <v>24</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>1</v>
+        <v>1801</v>
       </c>
       <c r="G268" t="s">
         <v>4824</v>
@@ -20542,7 +20564,7 @@
         <v>24</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>1</v>
+        <v>1801</v>
       </c>
       <c r="G269" t="s">
         <v>4824</v>
@@ -20559,7 +20581,7 @@
         <v>0</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>1</v>
+        <v>1809</v>
       </c>
       <c r="G270" t="s">
         <v>4761</v>
@@ -20576,7 +20598,7 @@
         <v>24</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>1</v>
+        <v>5028</v>
       </c>
       <c r="G271" t="s">
         <v>4824</v>
@@ -20593,7 +20615,7 @@
         <v>39</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>1</v>
+        <v>4592</v>
       </c>
       <c r="G272" t="s">
         <v>4782</v>
@@ -20610,7 +20632,7 @@
         <v>0</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>1</v>
+        <v>1889</v>
       </c>
       <c r="G273" t="s">
         <v>4756</v>
@@ -20627,7 +20649,7 @@
         <v>39</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>1</v>
+        <v>1889</v>
       </c>
       <c r="G274" t="s">
         <v>4782</v>
@@ -20644,7 +20666,7 @@
         <v>0</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>1</v>
+        <v>1929</v>
       </c>
       <c r="G275" t="s">
         <v>4756</v>
@@ -20661,7 +20683,7 @@
         <v>0</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>1</v>
+        <v>1929</v>
       </c>
       <c r="G276" t="s">
         <v>4787</v>
@@ -20678,7 +20700,7 @@
         <v>0</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>1</v>
+        <v>1932</v>
       </c>
       <c r="G277" t="s">
         <v>4787</v>
@@ -20695,7 +20717,7 @@
         <v>0</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>1</v>
+        <v>5029</v>
       </c>
       <c r="G278" t="s">
         <v>4838</v>
@@ -20712,7 +20734,7 @@
         <v>0</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>1</v>
+        <v>5030</v>
       </c>
       <c r="G279" t="s">
         <v>4787</v>
@@ -20728,7 +20750,7 @@
       <c r="C280" t="s">
         <v>0</v>
       </c>
-      <c r="D280" s="1" t="s">
+      <c r="D280" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G280" t="s">
@@ -20746,7 +20768,7 @@
         <v>0</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>1</v>
+        <v>2316</v>
       </c>
       <c r="G281" t="s">
         <v>4756</v>
@@ -20762,7 +20784,7 @@
       <c r="C282" t="s">
         <v>0</v>
       </c>
-      <c r="D282" s="1" t="s">
+      <c r="D282" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G282" t="s">
@@ -20780,7 +20802,7 @@
         <v>0</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>1</v>
+        <v>2316</v>
       </c>
       <c r="G283" t="s">
         <v>4838</v>
@@ -20796,7 +20818,7 @@
       <c r="C284" t="s">
         <v>0</v>
       </c>
-      <c r="D284" s="1" t="s">
+      <c r="D284" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G284" t="s">
@@ -20813,8 +20835,8 @@
       <c r="C285" t="s">
         <v>0</v>
       </c>
-      <c r="D285" s="1" t="s">
-        <v>1</v>
+      <c r="D285" s="5" t="s">
+        <v>3785</v>
       </c>
       <c r="G285" t="s">
         <v>4838</v>
@@ -20831,7 +20853,7 @@
         <v>24</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>1</v>
+        <v>2087</v>
       </c>
       <c r="G286" t="s">
         <v>4824</v>
@@ -20848,7 +20870,7 @@
         <v>24</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>1</v>
+        <v>2087</v>
       </c>
       <c r="G287" t="s">
         <v>4824</v>
@@ -20864,7 +20886,7 @@
       <c r="C288" t="s">
         <v>0</v>
       </c>
-      <c r="D288" s="1" t="s">
+      <c r="D288" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G288" t="s">
@@ -20881,7 +20903,7 @@
       <c r="C289" t="s">
         <v>39</v>
       </c>
-      <c r="D289" s="1" t="s">
+      <c r="D289" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G289" t="s">
@@ -20899,7 +20921,7 @@
         <v>0</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>1</v>
+        <v>2355</v>
       </c>
       <c r="G290" t="s">
         <v>4794</v>
@@ -20916,7 +20938,7 @@
         <v>39</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>1</v>
+        <v>2316</v>
       </c>
       <c r="G291" t="s">
         <v>4782</v>
@@ -20933,7 +20955,7 @@
         <v>39</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>1</v>
+        <v>2140</v>
       </c>
       <c r="G292" t="s">
         <v>4782</v>
@@ -20950,7 +20972,7 @@
         <v>39</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>1</v>
+        <v>5031</v>
       </c>
       <c r="G293" t="s">
         <v>4782</v>
@@ -20967,7 +20989,7 @@
         <v>39</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>1</v>
+        <v>2355</v>
       </c>
       <c r="G294" t="s">
         <v>4782</v>
@@ -20984,7 +21006,7 @@
         <v>39</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>1</v>
+        <v>2202</v>
       </c>
       <c r="G295" t="s">
         <v>4782</v>
@@ -21000,7 +21022,7 @@
       <c r="C296" t="s">
         <v>0</v>
       </c>
-      <c r="D296" s="1" t="s">
+      <c r="D296" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G296" t="s">
@@ -21017,7 +21039,7 @@
       <c r="C297" t="s">
         <v>0</v>
       </c>
-      <c r="D297" s="1" t="s">
+      <c r="D297" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G297" t="s">
@@ -21035,7 +21057,7 @@
         <v>0</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>1</v>
+        <v>2361</v>
       </c>
       <c r="G298" t="s">
         <v>4838</v>
@@ -21052,7 +21074,7 @@
         <v>0</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>1</v>
+        <v>2361</v>
       </c>
       <c r="G299" t="s">
         <v>4838</v>
@@ -21069,7 +21091,7 @@
         <v>0</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>1</v>
+        <v>2355</v>
       </c>
       <c r="G300" t="s">
         <v>4792</v>
@@ -21086,7 +21108,7 @@
         <v>39</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>1</v>
+        <v>2288</v>
       </c>
       <c r="G301" t="s">
         <v>4782</v>
@@ -21102,7 +21124,7 @@
       <c r="C302" t="s">
         <v>39</v>
       </c>
-      <c r="D302" s="1" t="s">
+      <c r="D302" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G302" t="s">
@@ -21120,7 +21142,7 @@
         <v>0</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>1</v>
+        <v>2297</v>
       </c>
       <c r="G303" t="s">
         <v>4756</v>
@@ -21137,7 +21159,7 @@
         <v>39</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>1</v>
+        <v>2297</v>
       </c>
       <c r="G304" t="s">
         <v>4782</v>
@@ -21154,7 +21176,7 @@
         <v>0</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>1</v>
+        <v>2297</v>
       </c>
       <c r="G305" t="s">
         <v>4787</v>
@@ -21170,7 +21192,7 @@
       <c r="C306" t="s">
         <v>0</v>
       </c>
-      <c r="D306" s="1" t="s">
+      <c r="D306" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G306" t="s">
@@ -21187,7 +21209,7 @@
       <c r="C307" t="s">
         <v>0</v>
       </c>
-      <c r="D307" s="1" t="s">
+      <c r="D307" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G307" t="s">
@@ -21204,7 +21226,7 @@
       <c r="C308" t="s">
         <v>0</v>
       </c>
-      <c r="D308" s="1" t="s">
+      <c r="D308" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G308" t="s">
@@ -21221,7 +21243,7 @@
       <c r="C309" t="s">
         <v>0</v>
       </c>
-      <c r="D309" s="1" t="s">
+      <c r="D309" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G309" t="s">
@@ -21239,7 +21261,7 @@
         <v>39</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>1</v>
+        <v>2411</v>
       </c>
       <c r="G310" t="s">
         <v>4782</v>
@@ -21256,7 +21278,7 @@
         <v>39</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>1</v>
+        <v>2448</v>
       </c>
       <c r="G311" t="s">
         <v>4782</v>
@@ -21273,7 +21295,7 @@
         <v>0</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>1</v>
+        <v>2410</v>
       </c>
       <c r="G312" t="s">
         <v>4842</v>
@@ -21290,7 +21312,7 @@
         <v>39</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>1</v>
+        <v>5032</v>
       </c>
       <c r="G313" t="s">
         <v>4782</v>
@@ -21307,7 +21329,7 @@
         <v>39</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>1</v>
+        <v>2449</v>
       </c>
       <c r="G314" t="s">
         <v>4782</v>
@@ -21324,7 +21346,7 @@
         <v>39</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>1</v>
+        <v>2394</v>
       </c>
       <c r="G315" t="s">
         <v>4782</v>
@@ -21341,7 +21363,7 @@
         <v>0</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>1</v>
+        <v>2451</v>
       </c>
       <c r="G316" t="s">
         <v>4837</v>
@@ -21358,7 +21380,7 @@
         <v>39</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>1</v>
+        <v>2451</v>
       </c>
       <c r="G317" t="s">
         <v>4837</v>
@@ -21375,7 +21397,7 @@
         <v>39</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>1</v>
+        <v>2453</v>
       </c>
       <c r="G318" t="s">
         <v>4782</v>
@@ -21392,7 +21414,7 @@
         <v>0</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>1</v>
+        <v>2842</v>
       </c>
       <c r="G319" t="s">
         <v>4838</v>
@@ -21408,7 +21430,7 @@
       <c r="C320" t="s">
         <v>275</v>
       </c>
-      <c r="D320" s="1" t="s">
+      <c r="D320" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -21422,7 +21444,7 @@
       <c r="C321" t="s">
         <v>932</v>
       </c>
-      <c r="D321" s="1" t="s">
+      <c r="D321" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G321" t="s">
@@ -21439,7 +21461,7 @@
       <c r="C322" t="s">
         <v>932</v>
       </c>
-      <c r="D322" s="1" t="s">
+      <c r="D322" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G322" t="s">
@@ -21457,7 +21479,7 @@
         <v>0</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>1</v>
+        <v>2556</v>
       </c>
       <c r="G323" t="s">
         <v>4767</v>
@@ -21474,7 +21496,7 @@
         <v>0</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>1</v>
+        <v>2841</v>
       </c>
       <c r="G324" t="s">
         <v>4756</v>
@@ -21491,7 +21513,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1</v>
+        <v>2842</v>
       </c>
       <c r="G325" t="s">
         <v>4797</v>
@@ -21508,7 +21530,7 @@
         <v>39</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>1</v>
+        <v>2842</v>
       </c>
       <c r="G326" t="s">
         <v>4797</v>
@@ -21524,7 +21546,7 @@
       <c r="C327" t="s">
         <v>0</v>
       </c>
-      <c r="D327" s="1" t="s">
+      <c r="D327" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G327" t="s">
@@ -21542,7 +21564,7 @@
         <v>0</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>1</v>
+        <v>2819</v>
       </c>
       <c r="G328" t="s">
         <v>4838</v>
@@ -21559,7 +21581,7 @@
         <v>0</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>1</v>
+        <v>2853</v>
       </c>
       <c r="G329" t="s">
         <v>4756</v>
@@ -21576,7 +21598,7 @@
         <v>0</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>1</v>
+        <v>2836</v>
       </c>
       <c r="G330" t="s">
         <v>4756</v>
@@ -21593,7 +21615,7 @@
         <v>0</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>1</v>
+        <v>2836</v>
       </c>
       <c r="G331" t="s">
         <v>4838</v>
@@ -21610,7 +21632,7 @@
         <v>0</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>1</v>
+        <v>2852</v>
       </c>
       <c r="G332" t="s">
         <v>4756</v>
@@ -21627,7 +21649,7 @@
         <v>39</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>1</v>
+        <v>2842</v>
       </c>
       <c r="G333" t="s">
         <v>4782</v>
@@ -21644,7 +21666,7 @@
         <v>39</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>1</v>
+        <v>5033</v>
       </c>
       <c r="G334" t="s">
         <v>4782</v>
@@ -22912,7 +22934,7 @@
       <c r="C409" t="s">
         <v>0</v>
       </c>
-      <c r="D409" s="1" t="s">
+      <c r="D409" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G409" t="s">
@@ -22949,7 +22971,7 @@
       <c r="C411" t="s">
         <v>0</v>
       </c>
-      <c r="D411" s="1" t="s">
+      <c r="D411" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G411" t="s">
@@ -22967,7 +22989,7 @@
         <v>0</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>1</v>
+        <v>4593</v>
       </c>
       <c r="G412" t="s">
         <v>4837</v>
@@ -22984,7 +23006,7 @@
         <v>39</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>1</v>
+        <v>4593</v>
       </c>
       <c r="G413" t="s">
         <v>4837</v>
@@ -23001,7 +23023,7 @@
         <v>0</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>1</v>
+        <v>5027</v>
       </c>
       <c r="G414" t="s">
         <v>4838</v>
@@ -23034,7 +23056,7 @@
       <c r="C416" t="s">
         <v>0</v>
       </c>
-      <c r="D416" s="1" t="s">
+      <c r="D416" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G416" t="s">
@@ -23102,7 +23124,7 @@
       <c r="C420" t="s">
         <v>0</v>
       </c>
-      <c r="D420" s="1" t="s">
+      <c r="D420" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G420" t="s">
@@ -23120,7 +23142,7 @@
         <v>0</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>1</v>
+        <v>3303</v>
       </c>
     </row>
     <row r="422" spans="1:7">
@@ -23419,7 +23441,7 @@
       <c r="C439" t="s">
         <v>39</v>
       </c>
-      <c r="D439" s="1" t="s">
+      <c r="D439" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G439" t="s">
@@ -23453,6 +23475,9 @@
       <c r="C441" t="s">
         <v>0</v>
       </c>
+      <c r="D441" s="5" t="s">
+        <v>4616</v>
+      </c>
     </row>
     <row r="442" spans="1:7">
       <c r="A442">
@@ -23532,9 +23557,7 @@
       <c r="C446" t="s">
         <v>39</v>
       </c>
-      <c r="D446" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="D446" s="5"/>
       <c r="G446" t="s">
         <v>4782</v>
       </c>
@@ -24210,7 +24233,7 @@
         <v>0</v>
       </c>
       <c r="D486" s="1" t="s">
-        <v>1</v>
+        <v>3806</v>
       </c>
       <c r="G486" t="s">
         <v>4756</v>
@@ -24227,7 +24250,7 @@
         <v>0</v>
       </c>
       <c r="D487" s="1" t="s">
-        <v>1</v>
+        <v>3762</v>
       </c>
       <c r="G487" t="s">
         <v>4756</v>
@@ -24244,7 +24267,7 @@
         <v>0</v>
       </c>
       <c r="D488" s="1" t="s">
-        <v>1</v>
+        <v>3807</v>
       </c>
       <c r="G488" t="s">
         <v>4756</v>
@@ -24260,7 +24283,7 @@
       <c r="C489" t="s">
         <v>2</v>
       </c>
-      <c r="D489" s="1" t="s">
+      <c r="D489" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G489" t="s">
@@ -24278,7 +24301,7 @@
         <v>39</v>
       </c>
       <c r="D490" s="1" t="s">
-        <v>1</v>
+        <v>3786</v>
       </c>
       <c r="G490" t="s">
         <v>4782</v>
@@ -24294,7 +24317,7 @@
       <c r="C491" t="s">
         <v>0</v>
       </c>
-      <c r="D491" s="1" t="s">
+      <c r="D491" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G491" t="s">
@@ -24311,7 +24334,7 @@
       <c r="C492" t="s">
         <v>0</v>
       </c>
-      <c r="D492" s="1" t="s">
+      <c r="D492" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G492" t="s">
@@ -24328,8 +24351,8 @@
       <c r="C493" t="s">
         <v>2</v>
       </c>
-      <c r="D493" s="1" t="s">
-        <v>1</v>
+      <c r="D493" s="5" t="s">
+        <v>3763</v>
       </c>
     </row>
     <row r="494" spans="1:7">
@@ -24360,7 +24383,7 @@
         <v>39</v>
       </c>
       <c r="D495" s="1" t="s">
-        <v>1</v>
+        <v>3291</v>
       </c>
       <c r="G495" t="s">
         <v>4782</v>
@@ -24376,7 +24399,7 @@
       <c r="C496" t="s">
         <v>2</v>
       </c>
-      <c r="D496" s="1" t="s">
+      <c r="D496" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G496" t="s">
@@ -24393,7 +24416,7 @@
       <c r="C497" t="s">
         <v>2</v>
       </c>
-      <c r="D497" s="1" t="s">
+      <c r="D497" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G497" t="s">
@@ -24410,7 +24433,7 @@
       <c r="C498" t="s">
         <v>0</v>
       </c>
-      <c r="D498" s="1" t="s">
+      <c r="D498" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -25547,7 +25570,7 @@
       <c r="C564" t="s">
         <v>0</v>
       </c>
-      <c r="D564" s="1" t="s">
+      <c r="D564" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G564" t="s">

</xml_diff>